<commit_message>
add scene, delete assets, fix error, add sound
</commit_message>
<xml_diff>
--- a/Assets/04Table/Fairytale.xlsx
+++ b/Assets/04Table/Fairytale.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cksgm\Unity\3D_Adventure\Assets\04Table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51DD7AF2-872D-410F-B560-3D91BC44DE73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A47A27-3447-4DF4-A8CB-5B6D4557EBF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="21480" windowHeight="13280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3270" yWindow="240" windowWidth="21480" windowHeight="13280" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ItemData" sheetId="1" r:id="rId1"/>
@@ -1291,7 +1291,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -4601,10 +4601,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -4697,6 +4697,91 @@
         <v>-7</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>75</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>-60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>40</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>-36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>-23</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.69972223043441772" right="0.69972223043441772" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>

</xml_diff>